<commit_message>
Adopt to nested ATD
</commit_message>
<xml_diff>
--- a/build_data_mlag.xlsx
+++ b/build_data_mlag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plavelle/Documents/Projects/GitLab Projects/cvp-excel-automation-demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mp/Programming/CVP/cvp-excel-automation-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD6552F-88C0-514C-9A4B-A1A5D9A72336}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FE74C5-E07E-DD40-8834-5CDC50844FB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="10260" windowWidth="29700" windowHeight="9200" xr2:uid="{E5C92443-CA13-0B47-BCB3-0563C90F2A27}"/>
+    <workbookView xWindow="820" yWindow="4120" windowWidth="39520" windowHeight="15340" xr2:uid="{E5C92443-CA13-0B47-BCB3-0563C90F2A27}"/>
   </bookViews>
   <sheets>
     <sheet name="device" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="139">
   <si>
     <t>status</t>
   </si>
@@ -395,39 +395,6 @@
     <t>172.16.200.1</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>10.83.30.63</t>
-  </si>
-  <si>
-    <t>10.83.30.64</t>
-  </si>
-  <si>
-    <t>10.83.30.67</t>
-  </si>
-  <si>
-    <t>10.83.30.68</t>
-  </si>
-  <si>
-    <t>50:2f:00:d2:1a:69</t>
-  </si>
-  <si>
-    <t>50:2f:00:da:92:3b</t>
-  </si>
-  <si>
-    <t>50:2f:00:f4:13:56</t>
-  </si>
-  <si>
-    <t>50:2f:00:03:9d:d2</t>
-  </si>
-  <si>
-    <t>50:2f:00:81:75:cf</t>
-  </si>
-  <si>
-    <t>50:2f:00:cb:cb:e4</t>
-  </si>
-  <si>
     <t>container</t>
   </si>
   <si>
@@ -443,17 +410,53 @@
     <t>ipv6_routing</t>
   </si>
   <si>
-    <t>10.83.30.69</t>
-  </si>
-  <si>
-    <t>10.83.30.75</t>
+    <t>00:1c:73:b0:c6:01</t>
+  </si>
+  <si>
+    <t>00:1c:73:b1:c6:01</t>
+  </si>
+  <si>
+    <t>00:1c:73:b2:c6:01</t>
+  </si>
+  <si>
+    <t>00:1c:73:b3:c6:01</t>
+  </si>
+  <si>
+    <t>00:1c:73:b4:c6:01</t>
+  </si>
+  <si>
+    <t>00:1c:73:b5:c6:01</t>
+  </si>
+  <si>
+    <t>192.168.0.10</t>
+  </si>
+  <si>
+    <t>192.168.0.11</t>
+  </si>
+  <si>
+    <t>192.168.0.12</t>
+  </si>
+  <si>
+    <t>192.168.0.13</t>
+  </si>
+  <si>
+    <t>192.168.0.14</t>
+  </si>
+  <si>
+    <t>192.168.0.15</t>
+  </si>
+  <si>
+    <t>Ethernet5</t>
+  </si>
+  <si>
+    <t>Ethernet6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -463,6 +466,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -810,7 +819,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8DCA0FF-5B85-8347-9E19-A812F32EF602}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -847,7 +858,7 @@
         <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>37</v>
@@ -888,7 +899,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>82</v>
@@ -897,7 +908,7 @@
         <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>38</v>
@@ -905,11 +916,11 @@
       <c r="G2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>121</v>
+      <c r="H2" t="s">
+        <v>131</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>50</v>
@@ -923,7 +934,7 @@
         <v>84</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>82</v>
@@ -932,7 +943,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
@@ -940,11 +951,11 @@
       <c r="G3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>122</v>
+      <c r="H3" t="s">
+        <v>132</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>51</v>
@@ -958,7 +969,7 @@
         <v>85</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>82</v>
@@ -967,7 +978,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>39</v>
@@ -975,11 +986,11 @@
       <c r="G4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>123</v>
+      <c r="H4" t="s">
+        <v>133</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>109</v>
@@ -1008,7 +1019,7 @@
         <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>82</v>
@@ -1017,7 +1028,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>39</v>
@@ -1025,11 +1036,11 @@
       <c r="G5" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>124</v>
+      <c r="H5" t="s">
+        <v>134</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>110</v>
@@ -1057,8 +1068,8 @@
       <c r="A6" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>128</v>
+      <c r="B6" t="s">
+        <v>129</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>82</v>
@@ -1067,7 +1078,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>39</v>
@@ -1075,11 +1086,11 @@
       <c r="G6" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>136</v>
+      <c r="H6" t="s">
+        <v>135</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>111</v>
@@ -1107,8 +1118,8 @@
       <c r="A7" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>127</v>
+      <c r="B7" t="s">
+        <v>130</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>82</v>
@@ -1117,7 +1128,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>39</v>
@@ -1125,11 +1136,11 @@
       <c r="G7" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>137</v>
+      <c r="H7" t="s">
+        <v>136</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>112</v>
@@ -1154,6 +1165,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1162,7 +1174,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B98C10-90BA-E941-9AB9-818A605AC062}">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1261,7 +1275,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -1276,7 +1290,7 @@
         <v>85</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>64</v>
@@ -1290,7 +1304,7 @@
         <v>83</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -1305,7 +1319,7 @@
         <v>86</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>65</v>
@@ -1319,7 +1333,7 @@
         <v>83</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
@@ -1334,7 +1348,7 @@
         <v>87</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>57</v>
@@ -1348,7 +1362,7 @@
         <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>3</v>
@@ -1363,7 +1377,7 @@
         <v>88</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>58</v>
@@ -1377,7 +1391,7 @@
         <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -1392,7 +1406,7 @@
         <v>85</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>66</v>
@@ -1406,7 +1420,7 @@
         <v>84</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>3</v>
@@ -1421,7 +1435,7 @@
         <v>86</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>67</v>
@@ -1435,7 +1449,7 @@
         <v>84</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>3</v>
@@ -1450,7 +1464,7 @@
         <v>87</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>59</v>
@@ -1464,7 +1478,7 @@
         <v>84</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>3</v>
@@ -1479,7 +1493,7 @@
         <v>88</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>60</v>
@@ -1493,7 +1507,7 @@
         <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>3</v>
@@ -1508,7 +1522,7 @@
         <v>83</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P12" s="4" t="s">
         <v>62</v>
@@ -1522,7 +1536,7 @@
         <v>85</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>3</v>
@@ -1537,7 +1551,7 @@
         <v>84</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>63</v>
@@ -1551,7 +1565,7 @@
         <v>85</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
@@ -1561,7 +1575,7 @@
         <v>86</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>103</v>
@@ -1575,7 +1589,7 @@
         <v>85</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
@@ -1584,7 +1598,7 @@
         <v>86</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>103</v>
@@ -1624,7 +1638,7 @@
         <v>86</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>3</v>
@@ -1639,7 +1653,7 @@
         <v>83</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>68</v>
@@ -1653,7 +1667,7 @@
         <v>86</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>3</v>
@@ -1668,7 +1682,7 @@
         <v>84</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>71</v>
@@ -1682,7 +1696,7 @@
         <v>86</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
@@ -1692,7 +1706,7 @@
         <v>85</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>103</v>
@@ -1706,7 +1720,7 @@
         <v>86</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
@@ -1715,7 +1729,7 @@
         <v>85</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>103</v>
@@ -1755,7 +1769,7 @@
         <v>87</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>3</v>
@@ -1770,7 +1784,7 @@
         <v>83</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P24" s="4" t="s">
         <v>69</v>
@@ -1784,7 +1798,7 @@
         <v>87</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>3</v>
@@ -1799,7 +1813,7 @@
         <v>84</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P25" s="4" t="s">
         <v>72</v>
@@ -1813,7 +1827,7 @@
         <v>87</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>3</v>
@@ -1823,7 +1837,7 @@
         <v>88</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>103</v>
@@ -1837,7 +1851,7 @@
         <v>87</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>3</v>
@@ -1846,7 +1860,7 @@
         <v>88</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="R27" s="2" t="s">
         <v>103</v>
@@ -1886,7 +1900,7 @@
         <v>88</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>3</v>
@@ -1901,7 +1915,7 @@
         <v>83</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="P30" s="4" t="s">
         <v>70</v>
@@ -1915,7 +1929,7 @@
         <v>88</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>3</v>
@@ -1930,7 +1944,7 @@
         <v>84</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="P31" s="4" t="s">
         <v>73</v>
@@ -1944,7 +1958,7 @@
         <v>88</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>3</v>
@@ -1954,7 +1968,7 @@
         <v>87</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R32" s="2" t="s">
         <v>103</v>
@@ -1968,7 +1982,7 @@
         <v>88</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>3</v>
@@ -1977,7 +1991,7 @@
         <v>87</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="R33" s="2" t="s">
         <v>103</v>
@@ -2014,6 +2028,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:V1" xr:uid="{0E7989B3-930E-8D40-9B4C-6E5B27C7988F}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2302,7 +2317,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -2317,7 +2332,7 @@
         <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -2337,7 +2352,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>96</v>
@@ -2363,7 +2378,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>116</v>
@@ -2410,7 +2425,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -2422,18 +2437,18 @@
         <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
         <v>94</v>
@@ -2448,7 +2463,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>94</v>
@@ -2463,7 +2478,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>99</v>

</xml_diff>